<commit_message>
file add 0318.txt, Update giziroku_2022
</commit_message>
<xml_diff>
--- a/議事録（LeotardHP）_2022.xlsx
+++ b/議事録（LeotardHP）_2022.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wud96\LeotardHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95638b460be2f97b/GitLocal/LeotardHP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C0F2FF-D024-4D1A-BB5A-E0948511814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{42C0F2FF-D024-4D1A-BB5A-E0948511814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7180DB44-E6FF-47E3-A604-F986479BD491}"/>
   <bookViews>
-    <workbookView xWindow="1212" yWindow="0" windowWidth="20988" windowHeight="12216" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0225" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="0317" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'0225'!$A$1:$G$60</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="96">
   <si>
     <t>打合せ議事録</t>
     <rPh sb="0" eb="2">
@@ -751,6 +752,221 @@
     </rPh>
     <rPh sb="10" eb="12">
       <t>キョウカ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>議事録</t>
+    <rPh sb="0" eb="3">
+      <t>ギジロク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>2022/0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> (木)　10:00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>~</t>
+    </r>
+    <rPh sb="12" eb="13">
+      <t>モク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>インフィニットソフト</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>参加者</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>イメージ合成ツールのコードをチェック</t>
+    <rPh sb="4" eb="6">
+      <t>ゴウセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>□なし　　■あり（index.html）</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>イメージ合成ツールのコードを全体的にチェック</t>
+    <rPh sb="4" eb="6">
+      <t>ゴウセイ</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>ゼンタイテキ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>コードチェック</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>リミットがある限り後に複雑になる可能性がある。</t>
+    <rPh sb="7" eb="8">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フクザツ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>カノウセイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>post_type</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>生地だけの識別子を割り当てるようにする。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>★</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>order by</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>登録する際に制限できるのか確認する。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>生地追加の場合の順番を考えて作成する。</t>
+    <rPh sb="0" eb="2">
+      <t>キジ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ジュンバン</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>カンガ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>一回で全部を読み込まない</t>
+    <rPh sb="0" eb="2">
+      <t>イッカイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ゼンブ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>→必要時だけ追加表示されるようにする。</t>
+    <rPh sb="6" eb="8">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>全域変数指定</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>DB接続は毎回しなくても問題なし</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>組み合わせによって結果が出るようにユニークな組み合わせを決定する。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>コードの</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>修整</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>DBの親構成確認</t>
+    <rPh sb="3" eb="4">
+      <t>オヤ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -762,7 +978,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd\(ddd\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -806,6 +1022,12 @@
       <name val="メイリオ"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1031,7 +1253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1176,6 +1398,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1460,335 +1685,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5CA1A9-61F5-4DC6-949C-8244E97F1666}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.1640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="4" width="2.3984375" style="3" customWidth="1"/>
+    <col min="1" max="4" width="2.4140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="60" style="3" customWidth="1"/>
-    <col min="6" max="6" width="3.19921875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.69921875" style="2" customWidth="1"/>
-    <col min="8" max="256" width="8.19921875" style="3"/>
-    <col min="257" max="260" width="2.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
+    <col min="8" max="256" width="8.1640625" style="3"/>
+    <col min="257" max="260" width="2.4140625" style="3" customWidth="1"/>
     <col min="261" max="261" width="60" style="3" customWidth="1"/>
-    <col min="262" max="262" width="3.19921875" style="3" customWidth="1"/>
-    <col min="263" max="263" width="6.69921875" style="3" customWidth="1"/>
-    <col min="264" max="512" width="8.19921875" style="3"/>
-    <col min="513" max="516" width="2.3984375" style="3" customWidth="1"/>
+    <col min="262" max="262" width="3.1640625" style="3" customWidth="1"/>
+    <col min="263" max="263" width="6.6640625" style="3" customWidth="1"/>
+    <col min="264" max="512" width="8.1640625" style="3"/>
+    <col min="513" max="516" width="2.4140625" style="3" customWidth="1"/>
     <col min="517" max="517" width="60" style="3" customWidth="1"/>
-    <col min="518" max="518" width="3.19921875" style="3" customWidth="1"/>
-    <col min="519" max="519" width="6.69921875" style="3" customWidth="1"/>
-    <col min="520" max="768" width="8.19921875" style="3"/>
-    <col min="769" max="772" width="2.3984375" style="3" customWidth="1"/>
+    <col min="518" max="518" width="3.1640625" style="3" customWidth="1"/>
+    <col min="519" max="519" width="6.6640625" style="3" customWidth="1"/>
+    <col min="520" max="768" width="8.1640625" style="3"/>
+    <col min="769" max="772" width="2.4140625" style="3" customWidth="1"/>
     <col min="773" max="773" width="60" style="3" customWidth="1"/>
-    <col min="774" max="774" width="3.19921875" style="3" customWidth="1"/>
-    <col min="775" max="775" width="6.69921875" style="3" customWidth="1"/>
-    <col min="776" max="1024" width="8.19921875" style="3"/>
-    <col min="1025" max="1028" width="2.3984375" style="3" customWidth="1"/>
+    <col min="774" max="774" width="3.1640625" style="3" customWidth="1"/>
+    <col min="775" max="775" width="6.6640625" style="3" customWidth="1"/>
+    <col min="776" max="1024" width="8.1640625" style="3"/>
+    <col min="1025" max="1028" width="2.4140625" style="3" customWidth="1"/>
     <col min="1029" max="1029" width="60" style="3" customWidth="1"/>
-    <col min="1030" max="1030" width="3.19921875" style="3" customWidth="1"/>
-    <col min="1031" max="1031" width="6.69921875" style="3" customWidth="1"/>
-    <col min="1032" max="1280" width="8.19921875" style="3"/>
-    <col min="1281" max="1284" width="2.3984375" style="3" customWidth="1"/>
+    <col min="1030" max="1030" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1031" max="1031" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1032" max="1280" width="8.1640625" style="3"/>
+    <col min="1281" max="1284" width="2.4140625" style="3" customWidth="1"/>
     <col min="1285" max="1285" width="60" style="3" customWidth="1"/>
-    <col min="1286" max="1286" width="3.19921875" style="3" customWidth="1"/>
-    <col min="1287" max="1287" width="6.69921875" style="3" customWidth="1"/>
-    <col min="1288" max="1536" width="8.19921875" style="3"/>
-    <col min="1537" max="1540" width="2.3984375" style="3" customWidth="1"/>
+    <col min="1286" max="1286" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1287" max="1287" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1288" max="1536" width="8.1640625" style="3"/>
+    <col min="1537" max="1540" width="2.4140625" style="3" customWidth="1"/>
     <col min="1541" max="1541" width="60" style="3" customWidth="1"/>
-    <col min="1542" max="1542" width="3.19921875" style="3" customWidth="1"/>
-    <col min="1543" max="1543" width="6.69921875" style="3" customWidth="1"/>
-    <col min="1544" max="1792" width="8.19921875" style="3"/>
-    <col min="1793" max="1796" width="2.3984375" style="3" customWidth="1"/>
+    <col min="1542" max="1542" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1543" max="1543" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1544" max="1792" width="8.1640625" style="3"/>
+    <col min="1793" max="1796" width="2.4140625" style="3" customWidth="1"/>
     <col min="1797" max="1797" width="60" style="3" customWidth="1"/>
-    <col min="1798" max="1798" width="3.19921875" style="3" customWidth="1"/>
-    <col min="1799" max="1799" width="6.69921875" style="3" customWidth="1"/>
-    <col min="1800" max="2048" width="8.19921875" style="3"/>
-    <col min="2049" max="2052" width="2.3984375" style="3" customWidth="1"/>
+    <col min="1798" max="1798" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1799" max="1799" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1800" max="2048" width="8.1640625" style="3"/>
+    <col min="2049" max="2052" width="2.4140625" style="3" customWidth="1"/>
     <col min="2053" max="2053" width="60" style="3" customWidth="1"/>
-    <col min="2054" max="2054" width="3.19921875" style="3" customWidth="1"/>
-    <col min="2055" max="2055" width="6.69921875" style="3" customWidth="1"/>
-    <col min="2056" max="2304" width="8.19921875" style="3"/>
-    <col min="2305" max="2308" width="2.3984375" style="3" customWidth="1"/>
+    <col min="2054" max="2054" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2055" max="2055" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2056" max="2304" width="8.1640625" style="3"/>
+    <col min="2305" max="2308" width="2.4140625" style="3" customWidth="1"/>
     <col min="2309" max="2309" width="60" style="3" customWidth="1"/>
-    <col min="2310" max="2310" width="3.19921875" style="3" customWidth="1"/>
-    <col min="2311" max="2311" width="6.69921875" style="3" customWidth="1"/>
-    <col min="2312" max="2560" width="8.19921875" style="3"/>
-    <col min="2561" max="2564" width="2.3984375" style="3" customWidth="1"/>
+    <col min="2310" max="2310" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2311" max="2311" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2312" max="2560" width="8.1640625" style="3"/>
+    <col min="2561" max="2564" width="2.4140625" style="3" customWidth="1"/>
     <col min="2565" max="2565" width="60" style="3" customWidth="1"/>
-    <col min="2566" max="2566" width="3.19921875" style="3" customWidth="1"/>
-    <col min="2567" max="2567" width="6.69921875" style="3" customWidth="1"/>
-    <col min="2568" max="2816" width="8.19921875" style="3"/>
-    <col min="2817" max="2820" width="2.3984375" style="3" customWidth="1"/>
+    <col min="2566" max="2566" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2567" max="2567" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2568" max="2816" width="8.1640625" style="3"/>
+    <col min="2817" max="2820" width="2.4140625" style="3" customWidth="1"/>
     <col min="2821" max="2821" width="60" style="3" customWidth="1"/>
-    <col min="2822" max="2822" width="3.19921875" style="3" customWidth="1"/>
-    <col min="2823" max="2823" width="6.69921875" style="3" customWidth="1"/>
-    <col min="2824" max="3072" width="8.19921875" style="3"/>
-    <col min="3073" max="3076" width="2.3984375" style="3" customWidth="1"/>
+    <col min="2822" max="2822" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2823" max="2823" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2824" max="3072" width="8.1640625" style="3"/>
+    <col min="3073" max="3076" width="2.4140625" style="3" customWidth="1"/>
     <col min="3077" max="3077" width="60" style="3" customWidth="1"/>
-    <col min="3078" max="3078" width="3.19921875" style="3" customWidth="1"/>
-    <col min="3079" max="3079" width="6.69921875" style="3" customWidth="1"/>
-    <col min="3080" max="3328" width="8.19921875" style="3"/>
-    <col min="3329" max="3332" width="2.3984375" style="3" customWidth="1"/>
+    <col min="3078" max="3078" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3079" max="3079" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3080" max="3328" width="8.1640625" style="3"/>
+    <col min="3329" max="3332" width="2.4140625" style="3" customWidth="1"/>
     <col min="3333" max="3333" width="60" style="3" customWidth="1"/>
-    <col min="3334" max="3334" width="3.19921875" style="3" customWidth="1"/>
-    <col min="3335" max="3335" width="6.69921875" style="3" customWidth="1"/>
-    <col min="3336" max="3584" width="8.19921875" style="3"/>
-    <col min="3585" max="3588" width="2.3984375" style="3" customWidth="1"/>
+    <col min="3334" max="3334" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3335" max="3335" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3336" max="3584" width="8.1640625" style="3"/>
+    <col min="3585" max="3588" width="2.4140625" style="3" customWidth="1"/>
     <col min="3589" max="3589" width="60" style="3" customWidth="1"/>
-    <col min="3590" max="3590" width="3.19921875" style="3" customWidth="1"/>
-    <col min="3591" max="3591" width="6.69921875" style="3" customWidth="1"/>
-    <col min="3592" max="3840" width="8.19921875" style="3"/>
-    <col min="3841" max="3844" width="2.3984375" style="3" customWidth="1"/>
+    <col min="3590" max="3590" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3591" max="3591" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3592" max="3840" width="8.1640625" style="3"/>
+    <col min="3841" max="3844" width="2.4140625" style="3" customWidth="1"/>
     <col min="3845" max="3845" width="60" style="3" customWidth="1"/>
-    <col min="3846" max="3846" width="3.19921875" style="3" customWidth="1"/>
-    <col min="3847" max="3847" width="6.69921875" style="3" customWidth="1"/>
-    <col min="3848" max="4096" width="8.19921875" style="3"/>
-    <col min="4097" max="4100" width="2.3984375" style="3" customWidth="1"/>
+    <col min="3846" max="3846" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3847" max="3847" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3848" max="4096" width="8.1640625" style="3"/>
+    <col min="4097" max="4100" width="2.4140625" style="3" customWidth="1"/>
     <col min="4101" max="4101" width="60" style="3" customWidth="1"/>
-    <col min="4102" max="4102" width="3.19921875" style="3" customWidth="1"/>
-    <col min="4103" max="4103" width="6.69921875" style="3" customWidth="1"/>
-    <col min="4104" max="4352" width="8.19921875" style="3"/>
-    <col min="4353" max="4356" width="2.3984375" style="3" customWidth="1"/>
+    <col min="4102" max="4102" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4103" max="4103" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4104" max="4352" width="8.1640625" style="3"/>
+    <col min="4353" max="4356" width="2.4140625" style="3" customWidth="1"/>
     <col min="4357" max="4357" width="60" style="3" customWidth="1"/>
-    <col min="4358" max="4358" width="3.19921875" style="3" customWidth="1"/>
-    <col min="4359" max="4359" width="6.69921875" style="3" customWidth="1"/>
-    <col min="4360" max="4608" width="8.19921875" style="3"/>
-    <col min="4609" max="4612" width="2.3984375" style="3" customWidth="1"/>
+    <col min="4358" max="4358" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4359" max="4359" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4360" max="4608" width="8.1640625" style="3"/>
+    <col min="4609" max="4612" width="2.4140625" style="3" customWidth="1"/>
     <col min="4613" max="4613" width="60" style="3" customWidth="1"/>
-    <col min="4614" max="4614" width="3.19921875" style="3" customWidth="1"/>
-    <col min="4615" max="4615" width="6.69921875" style="3" customWidth="1"/>
-    <col min="4616" max="4864" width="8.19921875" style="3"/>
-    <col min="4865" max="4868" width="2.3984375" style="3" customWidth="1"/>
+    <col min="4614" max="4614" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4615" max="4615" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4616" max="4864" width="8.1640625" style="3"/>
+    <col min="4865" max="4868" width="2.4140625" style="3" customWidth="1"/>
     <col min="4869" max="4869" width="60" style="3" customWidth="1"/>
-    <col min="4870" max="4870" width="3.19921875" style="3" customWidth="1"/>
-    <col min="4871" max="4871" width="6.69921875" style="3" customWidth="1"/>
-    <col min="4872" max="5120" width="8.19921875" style="3"/>
-    <col min="5121" max="5124" width="2.3984375" style="3" customWidth="1"/>
+    <col min="4870" max="4870" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4871" max="4871" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4872" max="5120" width="8.1640625" style="3"/>
+    <col min="5121" max="5124" width="2.4140625" style="3" customWidth="1"/>
     <col min="5125" max="5125" width="60" style="3" customWidth="1"/>
-    <col min="5126" max="5126" width="3.19921875" style="3" customWidth="1"/>
-    <col min="5127" max="5127" width="6.69921875" style="3" customWidth="1"/>
-    <col min="5128" max="5376" width="8.19921875" style="3"/>
-    <col min="5377" max="5380" width="2.3984375" style="3" customWidth="1"/>
+    <col min="5126" max="5126" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5127" max="5127" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5128" max="5376" width="8.1640625" style="3"/>
+    <col min="5377" max="5380" width="2.4140625" style="3" customWidth="1"/>
     <col min="5381" max="5381" width="60" style="3" customWidth="1"/>
-    <col min="5382" max="5382" width="3.19921875" style="3" customWidth="1"/>
-    <col min="5383" max="5383" width="6.69921875" style="3" customWidth="1"/>
-    <col min="5384" max="5632" width="8.19921875" style="3"/>
-    <col min="5633" max="5636" width="2.3984375" style="3" customWidth="1"/>
+    <col min="5382" max="5382" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5383" max="5383" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5384" max="5632" width="8.1640625" style="3"/>
+    <col min="5633" max="5636" width="2.4140625" style="3" customWidth="1"/>
     <col min="5637" max="5637" width="60" style="3" customWidth="1"/>
-    <col min="5638" max="5638" width="3.19921875" style="3" customWidth="1"/>
-    <col min="5639" max="5639" width="6.69921875" style="3" customWidth="1"/>
-    <col min="5640" max="5888" width="8.19921875" style="3"/>
-    <col min="5889" max="5892" width="2.3984375" style="3" customWidth="1"/>
+    <col min="5638" max="5638" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5639" max="5639" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5640" max="5888" width="8.1640625" style="3"/>
+    <col min="5889" max="5892" width="2.4140625" style="3" customWidth="1"/>
     <col min="5893" max="5893" width="60" style="3" customWidth="1"/>
-    <col min="5894" max="5894" width="3.19921875" style="3" customWidth="1"/>
-    <col min="5895" max="5895" width="6.69921875" style="3" customWidth="1"/>
-    <col min="5896" max="6144" width="8.19921875" style="3"/>
-    <col min="6145" max="6148" width="2.3984375" style="3" customWidth="1"/>
+    <col min="5894" max="5894" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5895" max="5895" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5896" max="6144" width="8.1640625" style="3"/>
+    <col min="6145" max="6148" width="2.4140625" style="3" customWidth="1"/>
     <col min="6149" max="6149" width="60" style="3" customWidth="1"/>
-    <col min="6150" max="6150" width="3.19921875" style="3" customWidth="1"/>
-    <col min="6151" max="6151" width="6.69921875" style="3" customWidth="1"/>
-    <col min="6152" max="6400" width="8.19921875" style="3"/>
-    <col min="6401" max="6404" width="2.3984375" style="3" customWidth="1"/>
+    <col min="6150" max="6150" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6151" max="6151" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6152" max="6400" width="8.1640625" style="3"/>
+    <col min="6401" max="6404" width="2.4140625" style="3" customWidth="1"/>
     <col min="6405" max="6405" width="60" style="3" customWidth="1"/>
-    <col min="6406" max="6406" width="3.19921875" style="3" customWidth="1"/>
-    <col min="6407" max="6407" width="6.69921875" style="3" customWidth="1"/>
-    <col min="6408" max="6656" width="8.19921875" style="3"/>
-    <col min="6657" max="6660" width="2.3984375" style="3" customWidth="1"/>
+    <col min="6406" max="6406" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6407" max="6407" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6408" max="6656" width="8.1640625" style="3"/>
+    <col min="6657" max="6660" width="2.4140625" style="3" customWidth="1"/>
     <col min="6661" max="6661" width="60" style="3" customWidth="1"/>
-    <col min="6662" max="6662" width="3.19921875" style="3" customWidth="1"/>
-    <col min="6663" max="6663" width="6.69921875" style="3" customWidth="1"/>
-    <col min="6664" max="6912" width="8.19921875" style="3"/>
-    <col min="6913" max="6916" width="2.3984375" style="3" customWidth="1"/>
+    <col min="6662" max="6662" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6663" max="6663" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6664" max="6912" width="8.1640625" style="3"/>
+    <col min="6913" max="6916" width="2.4140625" style="3" customWidth="1"/>
     <col min="6917" max="6917" width="60" style="3" customWidth="1"/>
-    <col min="6918" max="6918" width="3.19921875" style="3" customWidth="1"/>
-    <col min="6919" max="6919" width="6.69921875" style="3" customWidth="1"/>
-    <col min="6920" max="7168" width="8.19921875" style="3"/>
-    <col min="7169" max="7172" width="2.3984375" style="3" customWidth="1"/>
+    <col min="6918" max="6918" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6919" max="6919" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6920" max="7168" width="8.1640625" style="3"/>
+    <col min="7169" max="7172" width="2.4140625" style="3" customWidth="1"/>
     <col min="7173" max="7173" width="60" style="3" customWidth="1"/>
-    <col min="7174" max="7174" width="3.19921875" style="3" customWidth="1"/>
-    <col min="7175" max="7175" width="6.69921875" style="3" customWidth="1"/>
-    <col min="7176" max="7424" width="8.19921875" style="3"/>
-    <col min="7425" max="7428" width="2.3984375" style="3" customWidth="1"/>
+    <col min="7174" max="7174" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7175" max="7175" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7176" max="7424" width="8.1640625" style="3"/>
+    <col min="7425" max="7428" width="2.4140625" style="3" customWidth="1"/>
     <col min="7429" max="7429" width="60" style="3" customWidth="1"/>
-    <col min="7430" max="7430" width="3.19921875" style="3" customWidth="1"/>
-    <col min="7431" max="7431" width="6.69921875" style="3" customWidth="1"/>
-    <col min="7432" max="7680" width="8.19921875" style="3"/>
-    <col min="7681" max="7684" width="2.3984375" style="3" customWidth="1"/>
+    <col min="7430" max="7430" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7431" max="7431" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7432" max="7680" width="8.1640625" style="3"/>
+    <col min="7681" max="7684" width="2.4140625" style="3" customWidth="1"/>
     <col min="7685" max="7685" width="60" style="3" customWidth="1"/>
-    <col min="7686" max="7686" width="3.19921875" style="3" customWidth="1"/>
-    <col min="7687" max="7687" width="6.69921875" style="3" customWidth="1"/>
-    <col min="7688" max="7936" width="8.19921875" style="3"/>
-    <col min="7937" max="7940" width="2.3984375" style="3" customWidth="1"/>
+    <col min="7686" max="7686" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7687" max="7687" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7688" max="7936" width="8.1640625" style="3"/>
+    <col min="7937" max="7940" width="2.4140625" style="3" customWidth="1"/>
     <col min="7941" max="7941" width="60" style="3" customWidth="1"/>
-    <col min="7942" max="7942" width="3.19921875" style="3" customWidth="1"/>
-    <col min="7943" max="7943" width="6.69921875" style="3" customWidth="1"/>
-    <col min="7944" max="8192" width="8.19921875" style="3"/>
-    <col min="8193" max="8196" width="2.3984375" style="3" customWidth="1"/>
+    <col min="7942" max="7942" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7943" max="7943" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7944" max="8192" width="8.1640625" style="3"/>
+    <col min="8193" max="8196" width="2.4140625" style="3" customWidth="1"/>
     <col min="8197" max="8197" width="60" style="3" customWidth="1"/>
-    <col min="8198" max="8198" width="3.19921875" style="3" customWidth="1"/>
-    <col min="8199" max="8199" width="6.69921875" style="3" customWidth="1"/>
-    <col min="8200" max="8448" width="8.19921875" style="3"/>
-    <col min="8449" max="8452" width="2.3984375" style="3" customWidth="1"/>
+    <col min="8198" max="8198" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8199" max="8199" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8200" max="8448" width="8.1640625" style="3"/>
+    <col min="8449" max="8452" width="2.4140625" style="3" customWidth="1"/>
     <col min="8453" max="8453" width="60" style="3" customWidth="1"/>
-    <col min="8454" max="8454" width="3.19921875" style="3" customWidth="1"/>
-    <col min="8455" max="8455" width="6.69921875" style="3" customWidth="1"/>
-    <col min="8456" max="8704" width="8.19921875" style="3"/>
-    <col min="8705" max="8708" width="2.3984375" style="3" customWidth="1"/>
+    <col min="8454" max="8454" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8455" max="8455" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8456" max="8704" width="8.1640625" style="3"/>
+    <col min="8705" max="8708" width="2.4140625" style="3" customWidth="1"/>
     <col min="8709" max="8709" width="60" style="3" customWidth="1"/>
-    <col min="8710" max="8710" width="3.19921875" style="3" customWidth="1"/>
-    <col min="8711" max="8711" width="6.69921875" style="3" customWidth="1"/>
-    <col min="8712" max="8960" width="8.19921875" style="3"/>
-    <col min="8961" max="8964" width="2.3984375" style="3" customWidth="1"/>
+    <col min="8710" max="8710" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8711" max="8711" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8712" max="8960" width="8.1640625" style="3"/>
+    <col min="8961" max="8964" width="2.4140625" style="3" customWidth="1"/>
     <col min="8965" max="8965" width="60" style="3" customWidth="1"/>
-    <col min="8966" max="8966" width="3.19921875" style="3" customWidth="1"/>
-    <col min="8967" max="8967" width="6.69921875" style="3" customWidth="1"/>
-    <col min="8968" max="9216" width="8.19921875" style="3"/>
-    <col min="9217" max="9220" width="2.3984375" style="3" customWidth="1"/>
+    <col min="8966" max="8966" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8967" max="8967" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8968" max="9216" width="8.1640625" style="3"/>
+    <col min="9217" max="9220" width="2.4140625" style="3" customWidth="1"/>
     <col min="9221" max="9221" width="60" style="3" customWidth="1"/>
-    <col min="9222" max="9222" width="3.19921875" style="3" customWidth="1"/>
-    <col min="9223" max="9223" width="6.69921875" style="3" customWidth="1"/>
-    <col min="9224" max="9472" width="8.19921875" style="3"/>
-    <col min="9473" max="9476" width="2.3984375" style="3" customWidth="1"/>
+    <col min="9222" max="9222" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9223" max="9223" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9224" max="9472" width="8.1640625" style="3"/>
+    <col min="9473" max="9476" width="2.4140625" style="3" customWidth="1"/>
     <col min="9477" max="9477" width="60" style="3" customWidth="1"/>
-    <col min="9478" max="9478" width="3.19921875" style="3" customWidth="1"/>
-    <col min="9479" max="9479" width="6.69921875" style="3" customWidth="1"/>
-    <col min="9480" max="9728" width="8.19921875" style="3"/>
-    <col min="9729" max="9732" width="2.3984375" style="3" customWidth="1"/>
+    <col min="9478" max="9478" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9479" max="9479" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9480" max="9728" width="8.1640625" style="3"/>
+    <col min="9729" max="9732" width="2.4140625" style="3" customWidth="1"/>
     <col min="9733" max="9733" width="60" style="3" customWidth="1"/>
-    <col min="9734" max="9734" width="3.19921875" style="3" customWidth="1"/>
-    <col min="9735" max="9735" width="6.69921875" style="3" customWidth="1"/>
-    <col min="9736" max="9984" width="8.19921875" style="3"/>
-    <col min="9985" max="9988" width="2.3984375" style="3" customWidth="1"/>
+    <col min="9734" max="9734" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9735" max="9735" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9736" max="9984" width="8.1640625" style="3"/>
+    <col min="9985" max="9988" width="2.4140625" style="3" customWidth="1"/>
     <col min="9989" max="9989" width="60" style="3" customWidth="1"/>
-    <col min="9990" max="9990" width="3.19921875" style="3" customWidth="1"/>
-    <col min="9991" max="9991" width="6.69921875" style="3" customWidth="1"/>
-    <col min="9992" max="10240" width="8.19921875" style="3"/>
-    <col min="10241" max="10244" width="2.3984375" style="3" customWidth="1"/>
+    <col min="9990" max="9990" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9991" max="9991" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9992" max="10240" width="8.1640625" style="3"/>
+    <col min="10241" max="10244" width="2.4140625" style="3" customWidth="1"/>
     <col min="10245" max="10245" width="60" style="3" customWidth="1"/>
-    <col min="10246" max="10246" width="3.19921875" style="3" customWidth="1"/>
-    <col min="10247" max="10247" width="6.69921875" style="3" customWidth="1"/>
-    <col min="10248" max="10496" width="8.19921875" style="3"/>
-    <col min="10497" max="10500" width="2.3984375" style="3" customWidth="1"/>
+    <col min="10246" max="10246" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10247" max="10247" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10248" max="10496" width="8.1640625" style="3"/>
+    <col min="10497" max="10500" width="2.4140625" style="3" customWidth="1"/>
     <col min="10501" max="10501" width="60" style="3" customWidth="1"/>
-    <col min="10502" max="10502" width="3.19921875" style="3" customWidth="1"/>
-    <col min="10503" max="10503" width="6.69921875" style="3" customWidth="1"/>
-    <col min="10504" max="10752" width="8.19921875" style="3"/>
-    <col min="10753" max="10756" width="2.3984375" style="3" customWidth="1"/>
+    <col min="10502" max="10502" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10503" max="10503" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10504" max="10752" width="8.1640625" style="3"/>
+    <col min="10753" max="10756" width="2.4140625" style="3" customWidth="1"/>
     <col min="10757" max="10757" width="60" style="3" customWidth="1"/>
-    <col min="10758" max="10758" width="3.19921875" style="3" customWidth="1"/>
-    <col min="10759" max="10759" width="6.69921875" style="3" customWidth="1"/>
-    <col min="10760" max="11008" width="8.19921875" style="3"/>
-    <col min="11009" max="11012" width="2.3984375" style="3" customWidth="1"/>
+    <col min="10758" max="10758" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10759" max="10759" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10760" max="11008" width="8.1640625" style="3"/>
+    <col min="11009" max="11012" width="2.4140625" style="3" customWidth="1"/>
     <col min="11013" max="11013" width="60" style="3" customWidth="1"/>
-    <col min="11014" max="11014" width="3.19921875" style="3" customWidth="1"/>
-    <col min="11015" max="11015" width="6.69921875" style="3" customWidth="1"/>
-    <col min="11016" max="11264" width="8.19921875" style="3"/>
-    <col min="11265" max="11268" width="2.3984375" style="3" customWidth="1"/>
+    <col min="11014" max="11014" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11015" max="11015" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11016" max="11264" width="8.1640625" style="3"/>
+    <col min="11265" max="11268" width="2.4140625" style="3" customWidth="1"/>
     <col min="11269" max="11269" width="60" style="3" customWidth="1"/>
-    <col min="11270" max="11270" width="3.19921875" style="3" customWidth="1"/>
-    <col min="11271" max="11271" width="6.69921875" style="3" customWidth="1"/>
-    <col min="11272" max="11520" width="8.19921875" style="3"/>
-    <col min="11521" max="11524" width="2.3984375" style="3" customWidth="1"/>
+    <col min="11270" max="11270" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11271" max="11271" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11272" max="11520" width="8.1640625" style="3"/>
+    <col min="11521" max="11524" width="2.4140625" style="3" customWidth="1"/>
     <col min="11525" max="11525" width="60" style="3" customWidth="1"/>
-    <col min="11526" max="11526" width="3.19921875" style="3" customWidth="1"/>
-    <col min="11527" max="11527" width="6.69921875" style="3" customWidth="1"/>
-    <col min="11528" max="11776" width="8.19921875" style="3"/>
-    <col min="11777" max="11780" width="2.3984375" style="3" customWidth="1"/>
+    <col min="11526" max="11526" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11527" max="11527" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11528" max="11776" width="8.1640625" style="3"/>
+    <col min="11777" max="11780" width="2.4140625" style="3" customWidth="1"/>
     <col min="11781" max="11781" width="60" style="3" customWidth="1"/>
-    <col min="11782" max="11782" width="3.19921875" style="3" customWidth="1"/>
-    <col min="11783" max="11783" width="6.69921875" style="3" customWidth="1"/>
-    <col min="11784" max="12032" width="8.19921875" style="3"/>
-    <col min="12033" max="12036" width="2.3984375" style="3" customWidth="1"/>
+    <col min="11782" max="11782" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11783" max="11783" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11784" max="12032" width="8.1640625" style="3"/>
+    <col min="12033" max="12036" width="2.4140625" style="3" customWidth="1"/>
     <col min="12037" max="12037" width="60" style="3" customWidth="1"/>
-    <col min="12038" max="12038" width="3.19921875" style="3" customWidth="1"/>
-    <col min="12039" max="12039" width="6.69921875" style="3" customWidth="1"/>
-    <col min="12040" max="12288" width="8.19921875" style="3"/>
-    <col min="12289" max="12292" width="2.3984375" style="3" customWidth="1"/>
+    <col min="12038" max="12038" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12039" max="12039" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12040" max="12288" width="8.1640625" style="3"/>
+    <col min="12289" max="12292" width="2.4140625" style="3" customWidth="1"/>
     <col min="12293" max="12293" width="60" style="3" customWidth="1"/>
-    <col min="12294" max="12294" width="3.19921875" style="3" customWidth="1"/>
-    <col min="12295" max="12295" width="6.69921875" style="3" customWidth="1"/>
-    <col min="12296" max="12544" width="8.19921875" style="3"/>
-    <col min="12545" max="12548" width="2.3984375" style="3" customWidth="1"/>
+    <col min="12294" max="12294" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12295" max="12295" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12296" max="12544" width="8.1640625" style="3"/>
+    <col min="12545" max="12548" width="2.4140625" style="3" customWidth="1"/>
     <col min="12549" max="12549" width="60" style="3" customWidth="1"/>
-    <col min="12550" max="12550" width="3.19921875" style="3" customWidth="1"/>
-    <col min="12551" max="12551" width="6.69921875" style="3" customWidth="1"/>
-    <col min="12552" max="12800" width="8.19921875" style="3"/>
-    <col min="12801" max="12804" width="2.3984375" style="3" customWidth="1"/>
+    <col min="12550" max="12550" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12551" max="12551" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12552" max="12800" width="8.1640625" style="3"/>
+    <col min="12801" max="12804" width="2.4140625" style="3" customWidth="1"/>
     <col min="12805" max="12805" width="60" style="3" customWidth="1"/>
-    <col min="12806" max="12806" width="3.19921875" style="3" customWidth="1"/>
-    <col min="12807" max="12807" width="6.69921875" style="3" customWidth="1"/>
-    <col min="12808" max="13056" width="8.19921875" style="3"/>
-    <col min="13057" max="13060" width="2.3984375" style="3" customWidth="1"/>
+    <col min="12806" max="12806" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12807" max="12807" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12808" max="13056" width="8.1640625" style="3"/>
+    <col min="13057" max="13060" width="2.4140625" style="3" customWidth="1"/>
     <col min="13061" max="13061" width="60" style="3" customWidth="1"/>
-    <col min="13062" max="13062" width="3.19921875" style="3" customWidth="1"/>
-    <col min="13063" max="13063" width="6.69921875" style="3" customWidth="1"/>
-    <col min="13064" max="13312" width="8.19921875" style="3"/>
-    <col min="13313" max="13316" width="2.3984375" style="3" customWidth="1"/>
+    <col min="13062" max="13062" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13063" max="13063" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13064" max="13312" width="8.1640625" style="3"/>
+    <col min="13313" max="13316" width="2.4140625" style="3" customWidth="1"/>
     <col min="13317" max="13317" width="60" style="3" customWidth="1"/>
-    <col min="13318" max="13318" width="3.19921875" style="3" customWidth="1"/>
-    <col min="13319" max="13319" width="6.69921875" style="3" customWidth="1"/>
-    <col min="13320" max="13568" width="8.19921875" style="3"/>
-    <col min="13569" max="13572" width="2.3984375" style="3" customWidth="1"/>
+    <col min="13318" max="13318" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13319" max="13319" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13320" max="13568" width="8.1640625" style="3"/>
+    <col min="13569" max="13572" width="2.4140625" style="3" customWidth="1"/>
     <col min="13573" max="13573" width="60" style="3" customWidth="1"/>
-    <col min="13574" max="13574" width="3.19921875" style="3" customWidth="1"/>
-    <col min="13575" max="13575" width="6.69921875" style="3" customWidth="1"/>
-    <col min="13576" max="13824" width="8.19921875" style="3"/>
-    <col min="13825" max="13828" width="2.3984375" style="3" customWidth="1"/>
+    <col min="13574" max="13574" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13575" max="13575" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13576" max="13824" width="8.1640625" style="3"/>
+    <col min="13825" max="13828" width="2.4140625" style="3" customWidth="1"/>
     <col min="13829" max="13829" width="60" style="3" customWidth="1"/>
-    <col min="13830" max="13830" width="3.19921875" style="3" customWidth="1"/>
-    <col min="13831" max="13831" width="6.69921875" style="3" customWidth="1"/>
-    <col min="13832" max="14080" width="8.19921875" style="3"/>
-    <col min="14081" max="14084" width="2.3984375" style="3" customWidth="1"/>
+    <col min="13830" max="13830" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13831" max="13831" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13832" max="14080" width="8.1640625" style="3"/>
+    <col min="14081" max="14084" width="2.4140625" style="3" customWidth="1"/>
     <col min="14085" max="14085" width="60" style="3" customWidth="1"/>
-    <col min="14086" max="14086" width="3.19921875" style="3" customWidth="1"/>
-    <col min="14087" max="14087" width="6.69921875" style="3" customWidth="1"/>
-    <col min="14088" max="14336" width="8.19921875" style="3"/>
-    <col min="14337" max="14340" width="2.3984375" style="3" customWidth="1"/>
+    <col min="14086" max="14086" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14087" max="14087" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14088" max="14336" width="8.1640625" style="3"/>
+    <col min="14337" max="14340" width="2.4140625" style="3" customWidth="1"/>
     <col min="14341" max="14341" width="60" style="3" customWidth="1"/>
-    <col min="14342" max="14342" width="3.19921875" style="3" customWidth="1"/>
-    <col min="14343" max="14343" width="6.69921875" style="3" customWidth="1"/>
-    <col min="14344" max="14592" width="8.19921875" style="3"/>
-    <col min="14593" max="14596" width="2.3984375" style="3" customWidth="1"/>
+    <col min="14342" max="14342" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14343" max="14343" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14344" max="14592" width="8.1640625" style="3"/>
+    <col min="14593" max="14596" width="2.4140625" style="3" customWidth="1"/>
     <col min="14597" max="14597" width="60" style="3" customWidth="1"/>
-    <col min="14598" max="14598" width="3.19921875" style="3" customWidth="1"/>
-    <col min="14599" max="14599" width="6.69921875" style="3" customWidth="1"/>
-    <col min="14600" max="14848" width="8.19921875" style="3"/>
-    <col min="14849" max="14852" width="2.3984375" style="3" customWidth="1"/>
+    <col min="14598" max="14598" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14599" max="14599" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14600" max="14848" width="8.1640625" style="3"/>
+    <col min="14849" max="14852" width="2.4140625" style="3" customWidth="1"/>
     <col min="14853" max="14853" width="60" style="3" customWidth="1"/>
-    <col min="14854" max="14854" width="3.19921875" style="3" customWidth="1"/>
-    <col min="14855" max="14855" width="6.69921875" style="3" customWidth="1"/>
-    <col min="14856" max="15104" width="8.19921875" style="3"/>
-    <col min="15105" max="15108" width="2.3984375" style="3" customWidth="1"/>
+    <col min="14854" max="14854" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14855" max="14855" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14856" max="15104" width="8.1640625" style="3"/>
+    <col min="15105" max="15108" width="2.4140625" style="3" customWidth="1"/>
     <col min="15109" max="15109" width="60" style="3" customWidth="1"/>
-    <col min="15110" max="15110" width="3.19921875" style="3" customWidth="1"/>
-    <col min="15111" max="15111" width="6.69921875" style="3" customWidth="1"/>
-    <col min="15112" max="15360" width="8.19921875" style="3"/>
-    <col min="15361" max="15364" width="2.3984375" style="3" customWidth="1"/>
+    <col min="15110" max="15110" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15111" max="15111" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15112" max="15360" width="8.1640625" style="3"/>
+    <col min="15361" max="15364" width="2.4140625" style="3" customWidth="1"/>
     <col min="15365" max="15365" width="60" style="3" customWidth="1"/>
-    <col min="15366" max="15366" width="3.19921875" style="3" customWidth="1"/>
-    <col min="15367" max="15367" width="6.69921875" style="3" customWidth="1"/>
-    <col min="15368" max="15616" width="8.19921875" style="3"/>
-    <col min="15617" max="15620" width="2.3984375" style="3" customWidth="1"/>
+    <col min="15366" max="15366" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15367" max="15367" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15368" max="15616" width="8.1640625" style="3"/>
+    <col min="15617" max="15620" width="2.4140625" style="3" customWidth="1"/>
     <col min="15621" max="15621" width="60" style="3" customWidth="1"/>
-    <col min="15622" max="15622" width="3.19921875" style="3" customWidth="1"/>
-    <col min="15623" max="15623" width="6.69921875" style="3" customWidth="1"/>
-    <col min="15624" max="15872" width="8.19921875" style="3"/>
-    <col min="15873" max="15876" width="2.3984375" style="3" customWidth="1"/>
+    <col min="15622" max="15622" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15623" max="15623" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15624" max="15872" width="8.1640625" style="3"/>
+    <col min="15873" max="15876" width="2.4140625" style="3" customWidth="1"/>
     <col min="15877" max="15877" width="60" style="3" customWidth="1"/>
-    <col min="15878" max="15878" width="3.19921875" style="3" customWidth="1"/>
-    <col min="15879" max="15879" width="6.69921875" style="3" customWidth="1"/>
-    <col min="15880" max="16128" width="8.19921875" style="3"/>
-    <col min="16129" max="16132" width="2.3984375" style="3" customWidth="1"/>
+    <col min="15878" max="15878" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15879" max="15879" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15880" max="16128" width="8.1640625" style="3"/>
+    <col min="16129" max="16132" width="2.4140625" style="3" customWidth="1"/>
     <col min="16133" max="16133" width="60" style="3" customWidth="1"/>
-    <col min="16134" max="16134" width="3.19921875" style="3" customWidth="1"/>
-    <col min="16135" max="16135" width="6.69921875" style="3" customWidth="1"/>
-    <col min="16136" max="16384" width="8.19921875" style="3"/>
+    <col min="16134" max="16134" width="3.1640625" style="3" customWidth="1"/>
+    <col min="16135" max="16135" width="6.6640625" style="3" customWidth="1"/>
+    <col min="16136" max="16384" width="8.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.6">
+    <row r="1" spans="1:7" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1905,7 +2130,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" s="9" customFormat="1" ht="15.6" thickBot="1">
+    <row r="10" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1939,7 +2164,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" s="9" customFormat="1" ht="15.6" thickBot="1">
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -2479,7 +2704,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" s="9" customFormat="1" ht="15.6" thickBot="1">
+    <row r="52" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
       <c r="A52" s="23"/>
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
@@ -2620,6 +2845,795 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785AD88A-8F29-48D7-B33D-53D7BFDEF27B}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.1640625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="4" width="2.4140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
+    <col min="8" max="256" width="8.1640625" style="3"/>
+    <col min="257" max="260" width="2.4140625" style="3" customWidth="1"/>
+    <col min="261" max="261" width="60" style="3" customWidth="1"/>
+    <col min="262" max="262" width="3.1640625" style="3" customWidth="1"/>
+    <col min="263" max="263" width="6.6640625" style="3" customWidth="1"/>
+    <col min="264" max="512" width="8.1640625" style="3"/>
+    <col min="513" max="516" width="2.4140625" style="3" customWidth="1"/>
+    <col min="517" max="517" width="60" style="3" customWidth="1"/>
+    <col min="518" max="518" width="3.1640625" style="3" customWidth="1"/>
+    <col min="519" max="519" width="6.6640625" style="3" customWidth="1"/>
+    <col min="520" max="768" width="8.1640625" style="3"/>
+    <col min="769" max="772" width="2.4140625" style="3" customWidth="1"/>
+    <col min="773" max="773" width="60" style="3" customWidth="1"/>
+    <col min="774" max="774" width="3.1640625" style="3" customWidth="1"/>
+    <col min="775" max="775" width="6.6640625" style="3" customWidth="1"/>
+    <col min="776" max="1024" width="8.1640625" style="3"/>
+    <col min="1025" max="1028" width="2.4140625" style="3" customWidth="1"/>
+    <col min="1029" max="1029" width="60" style="3" customWidth="1"/>
+    <col min="1030" max="1030" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1031" max="1031" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1032" max="1280" width="8.1640625" style="3"/>
+    <col min="1281" max="1284" width="2.4140625" style="3" customWidth="1"/>
+    <col min="1285" max="1285" width="60" style="3" customWidth="1"/>
+    <col min="1286" max="1286" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1287" max="1287" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1288" max="1536" width="8.1640625" style="3"/>
+    <col min="1537" max="1540" width="2.4140625" style="3" customWidth="1"/>
+    <col min="1541" max="1541" width="60" style="3" customWidth="1"/>
+    <col min="1542" max="1542" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1543" max="1543" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1544" max="1792" width="8.1640625" style="3"/>
+    <col min="1793" max="1796" width="2.4140625" style="3" customWidth="1"/>
+    <col min="1797" max="1797" width="60" style="3" customWidth="1"/>
+    <col min="1798" max="1798" width="3.1640625" style="3" customWidth="1"/>
+    <col min="1799" max="1799" width="6.6640625" style="3" customWidth="1"/>
+    <col min="1800" max="2048" width="8.1640625" style="3"/>
+    <col min="2049" max="2052" width="2.4140625" style="3" customWidth="1"/>
+    <col min="2053" max="2053" width="60" style="3" customWidth="1"/>
+    <col min="2054" max="2054" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2055" max="2055" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2056" max="2304" width="8.1640625" style="3"/>
+    <col min="2305" max="2308" width="2.4140625" style="3" customWidth="1"/>
+    <col min="2309" max="2309" width="60" style="3" customWidth="1"/>
+    <col min="2310" max="2310" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2311" max="2311" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2312" max="2560" width="8.1640625" style="3"/>
+    <col min="2561" max="2564" width="2.4140625" style="3" customWidth="1"/>
+    <col min="2565" max="2565" width="60" style="3" customWidth="1"/>
+    <col min="2566" max="2566" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2567" max="2567" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2568" max="2816" width="8.1640625" style="3"/>
+    <col min="2817" max="2820" width="2.4140625" style="3" customWidth="1"/>
+    <col min="2821" max="2821" width="60" style="3" customWidth="1"/>
+    <col min="2822" max="2822" width="3.1640625" style="3" customWidth="1"/>
+    <col min="2823" max="2823" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2824" max="3072" width="8.1640625" style="3"/>
+    <col min="3073" max="3076" width="2.4140625" style="3" customWidth="1"/>
+    <col min="3077" max="3077" width="60" style="3" customWidth="1"/>
+    <col min="3078" max="3078" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3079" max="3079" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3080" max="3328" width="8.1640625" style="3"/>
+    <col min="3329" max="3332" width="2.4140625" style="3" customWidth="1"/>
+    <col min="3333" max="3333" width="60" style="3" customWidth="1"/>
+    <col min="3334" max="3334" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3335" max="3335" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3336" max="3584" width="8.1640625" style="3"/>
+    <col min="3585" max="3588" width="2.4140625" style="3" customWidth="1"/>
+    <col min="3589" max="3589" width="60" style="3" customWidth="1"/>
+    <col min="3590" max="3590" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3591" max="3591" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3592" max="3840" width="8.1640625" style="3"/>
+    <col min="3841" max="3844" width="2.4140625" style="3" customWidth="1"/>
+    <col min="3845" max="3845" width="60" style="3" customWidth="1"/>
+    <col min="3846" max="3846" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3847" max="3847" width="6.6640625" style="3" customWidth="1"/>
+    <col min="3848" max="4096" width="8.1640625" style="3"/>
+    <col min="4097" max="4100" width="2.4140625" style="3" customWidth="1"/>
+    <col min="4101" max="4101" width="60" style="3" customWidth="1"/>
+    <col min="4102" max="4102" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4103" max="4103" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4104" max="4352" width="8.1640625" style="3"/>
+    <col min="4353" max="4356" width="2.4140625" style="3" customWidth="1"/>
+    <col min="4357" max="4357" width="60" style="3" customWidth="1"/>
+    <col min="4358" max="4358" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4359" max="4359" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4360" max="4608" width="8.1640625" style="3"/>
+    <col min="4609" max="4612" width="2.4140625" style="3" customWidth="1"/>
+    <col min="4613" max="4613" width="60" style="3" customWidth="1"/>
+    <col min="4614" max="4614" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4615" max="4615" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4616" max="4864" width="8.1640625" style="3"/>
+    <col min="4865" max="4868" width="2.4140625" style="3" customWidth="1"/>
+    <col min="4869" max="4869" width="60" style="3" customWidth="1"/>
+    <col min="4870" max="4870" width="3.1640625" style="3" customWidth="1"/>
+    <col min="4871" max="4871" width="6.6640625" style="3" customWidth="1"/>
+    <col min="4872" max="5120" width="8.1640625" style="3"/>
+    <col min="5121" max="5124" width="2.4140625" style="3" customWidth="1"/>
+    <col min="5125" max="5125" width="60" style="3" customWidth="1"/>
+    <col min="5126" max="5126" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5127" max="5127" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5128" max="5376" width="8.1640625" style="3"/>
+    <col min="5377" max="5380" width="2.4140625" style="3" customWidth="1"/>
+    <col min="5381" max="5381" width="60" style="3" customWidth="1"/>
+    <col min="5382" max="5382" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5383" max="5383" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5384" max="5632" width="8.1640625" style="3"/>
+    <col min="5633" max="5636" width="2.4140625" style="3" customWidth="1"/>
+    <col min="5637" max="5637" width="60" style="3" customWidth="1"/>
+    <col min="5638" max="5638" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5639" max="5639" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5640" max="5888" width="8.1640625" style="3"/>
+    <col min="5889" max="5892" width="2.4140625" style="3" customWidth="1"/>
+    <col min="5893" max="5893" width="60" style="3" customWidth="1"/>
+    <col min="5894" max="5894" width="3.1640625" style="3" customWidth="1"/>
+    <col min="5895" max="5895" width="6.6640625" style="3" customWidth="1"/>
+    <col min="5896" max="6144" width="8.1640625" style="3"/>
+    <col min="6145" max="6148" width="2.4140625" style="3" customWidth="1"/>
+    <col min="6149" max="6149" width="60" style="3" customWidth="1"/>
+    <col min="6150" max="6150" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6151" max="6151" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6152" max="6400" width="8.1640625" style="3"/>
+    <col min="6401" max="6404" width="2.4140625" style="3" customWidth="1"/>
+    <col min="6405" max="6405" width="60" style="3" customWidth="1"/>
+    <col min="6406" max="6406" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6407" max="6407" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6408" max="6656" width="8.1640625" style="3"/>
+    <col min="6657" max="6660" width="2.4140625" style="3" customWidth="1"/>
+    <col min="6661" max="6661" width="60" style="3" customWidth="1"/>
+    <col min="6662" max="6662" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6663" max="6663" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6664" max="6912" width="8.1640625" style="3"/>
+    <col min="6913" max="6916" width="2.4140625" style="3" customWidth="1"/>
+    <col min="6917" max="6917" width="60" style="3" customWidth="1"/>
+    <col min="6918" max="6918" width="3.1640625" style="3" customWidth="1"/>
+    <col min="6919" max="6919" width="6.6640625" style="3" customWidth="1"/>
+    <col min="6920" max="7168" width="8.1640625" style="3"/>
+    <col min="7169" max="7172" width="2.4140625" style="3" customWidth="1"/>
+    <col min="7173" max="7173" width="60" style="3" customWidth="1"/>
+    <col min="7174" max="7174" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7175" max="7175" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7176" max="7424" width="8.1640625" style="3"/>
+    <col min="7425" max="7428" width="2.4140625" style="3" customWidth="1"/>
+    <col min="7429" max="7429" width="60" style="3" customWidth="1"/>
+    <col min="7430" max="7430" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7431" max="7431" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7432" max="7680" width="8.1640625" style="3"/>
+    <col min="7681" max="7684" width="2.4140625" style="3" customWidth="1"/>
+    <col min="7685" max="7685" width="60" style="3" customWidth="1"/>
+    <col min="7686" max="7686" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7687" max="7687" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7688" max="7936" width="8.1640625" style="3"/>
+    <col min="7937" max="7940" width="2.4140625" style="3" customWidth="1"/>
+    <col min="7941" max="7941" width="60" style="3" customWidth="1"/>
+    <col min="7942" max="7942" width="3.1640625" style="3" customWidth="1"/>
+    <col min="7943" max="7943" width="6.6640625" style="3" customWidth="1"/>
+    <col min="7944" max="8192" width="8.1640625" style="3"/>
+    <col min="8193" max="8196" width="2.4140625" style="3" customWidth="1"/>
+    <col min="8197" max="8197" width="60" style="3" customWidth="1"/>
+    <col min="8198" max="8198" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8199" max="8199" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8200" max="8448" width="8.1640625" style="3"/>
+    <col min="8449" max="8452" width="2.4140625" style="3" customWidth="1"/>
+    <col min="8453" max="8453" width="60" style="3" customWidth="1"/>
+    <col min="8454" max="8454" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8455" max="8455" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8456" max="8704" width="8.1640625" style="3"/>
+    <col min="8705" max="8708" width="2.4140625" style="3" customWidth="1"/>
+    <col min="8709" max="8709" width="60" style="3" customWidth="1"/>
+    <col min="8710" max="8710" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8711" max="8711" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8712" max="8960" width="8.1640625" style="3"/>
+    <col min="8961" max="8964" width="2.4140625" style="3" customWidth="1"/>
+    <col min="8965" max="8965" width="60" style="3" customWidth="1"/>
+    <col min="8966" max="8966" width="3.1640625" style="3" customWidth="1"/>
+    <col min="8967" max="8967" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8968" max="9216" width="8.1640625" style="3"/>
+    <col min="9217" max="9220" width="2.4140625" style="3" customWidth="1"/>
+    <col min="9221" max="9221" width="60" style="3" customWidth="1"/>
+    <col min="9222" max="9222" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9223" max="9223" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9224" max="9472" width="8.1640625" style="3"/>
+    <col min="9473" max="9476" width="2.4140625" style="3" customWidth="1"/>
+    <col min="9477" max="9477" width="60" style="3" customWidth="1"/>
+    <col min="9478" max="9478" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9479" max="9479" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9480" max="9728" width="8.1640625" style="3"/>
+    <col min="9729" max="9732" width="2.4140625" style="3" customWidth="1"/>
+    <col min="9733" max="9733" width="60" style="3" customWidth="1"/>
+    <col min="9734" max="9734" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9735" max="9735" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9736" max="9984" width="8.1640625" style="3"/>
+    <col min="9985" max="9988" width="2.4140625" style="3" customWidth="1"/>
+    <col min="9989" max="9989" width="60" style="3" customWidth="1"/>
+    <col min="9990" max="9990" width="3.1640625" style="3" customWidth="1"/>
+    <col min="9991" max="9991" width="6.6640625" style="3" customWidth="1"/>
+    <col min="9992" max="10240" width="8.1640625" style="3"/>
+    <col min="10241" max="10244" width="2.4140625" style="3" customWidth="1"/>
+    <col min="10245" max="10245" width="60" style="3" customWidth="1"/>
+    <col min="10246" max="10246" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10247" max="10247" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10248" max="10496" width="8.1640625" style="3"/>
+    <col min="10497" max="10500" width="2.4140625" style="3" customWidth="1"/>
+    <col min="10501" max="10501" width="60" style="3" customWidth="1"/>
+    <col min="10502" max="10502" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10503" max="10503" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10504" max="10752" width="8.1640625" style="3"/>
+    <col min="10753" max="10756" width="2.4140625" style="3" customWidth="1"/>
+    <col min="10757" max="10757" width="60" style="3" customWidth="1"/>
+    <col min="10758" max="10758" width="3.1640625" style="3" customWidth="1"/>
+    <col min="10759" max="10759" width="6.6640625" style="3" customWidth="1"/>
+    <col min="10760" max="11008" width="8.1640625" style="3"/>
+    <col min="11009" max="11012" width="2.4140625" style="3" customWidth="1"/>
+    <col min="11013" max="11013" width="60" style="3" customWidth="1"/>
+    <col min="11014" max="11014" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11015" max="11015" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11016" max="11264" width="8.1640625" style="3"/>
+    <col min="11265" max="11268" width="2.4140625" style="3" customWidth="1"/>
+    <col min="11269" max="11269" width="60" style="3" customWidth="1"/>
+    <col min="11270" max="11270" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11271" max="11271" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11272" max="11520" width="8.1640625" style="3"/>
+    <col min="11521" max="11524" width="2.4140625" style="3" customWidth="1"/>
+    <col min="11525" max="11525" width="60" style="3" customWidth="1"/>
+    <col min="11526" max="11526" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11527" max="11527" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11528" max="11776" width="8.1640625" style="3"/>
+    <col min="11777" max="11780" width="2.4140625" style="3" customWidth="1"/>
+    <col min="11781" max="11781" width="60" style="3" customWidth="1"/>
+    <col min="11782" max="11782" width="3.1640625" style="3" customWidth="1"/>
+    <col min="11783" max="11783" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11784" max="12032" width="8.1640625" style="3"/>
+    <col min="12033" max="12036" width="2.4140625" style="3" customWidth="1"/>
+    <col min="12037" max="12037" width="60" style="3" customWidth="1"/>
+    <col min="12038" max="12038" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12039" max="12039" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12040" max="12288" width="8.1640625" style="3"/>
+    <col min="12289" max="12292" width="2.4140625" style="3" customWidth="1"/>
+    <col min="12293" max="12293" width="60" style="3" customWidth="1"/>
+    <col min="12294" max="12294" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12295" max="12295" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12296" max="12544" width="8.1640625" style="3"/>
+    <col min="12545" max="12548" width="2.4140625" style="3" customWidth="1"/>
+    <col min="12549" max="12549" width="60" style="3" customWidth="1"/>
+    <col min="12550" max="12550" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12551" max="12551" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12552" max="12800" width="8.1640625" style="3"/>
+    <col min="12801" max="12804" width="2.4140625" style="3" customWidth="1"/>
+    <col min="12805" max="12805" width="60" style="3" customWidth="1"/>
+    <col min="12806" max="12806" width="3.1640625" style="3" customWidth="1"/>
+    <col min="12807" max="12807" width="6.6640625" style="3" customWidth="1"/>
+    <col min="12808" max="13056" width="8.1640625" style="3"/>
+    <col min="13057" max="13060" width="2.4140625" style="3" customWidth="1"/>
+    <col min="13061" max="13061" width="60" style="3" customWidth="1"/>
+    <col min="13062" max="13062" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13063" max="13063" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13064" max="13312" width="8.1640625" style="3"/>
+    <col min="13313" max="13316" width="2.4140625" style="3" customWidth="1"/>
+    <col min="13317" max="13317" width="60" style="3" customWidth="1"/>
+    <col min="13318" max="13318" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13319" max="13319" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13320" max="13568" width="8.1640625" style="3"/>
+    <col min="13569" max="13572" width="2.4140625" style="3" customWidth="1"/>
+    <col min="13573" max="13573" width="60" style="3" customWidth="1"/>
+    <col min="13574" max="13574" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13575" max="13575" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13576" max="13824" width="8.1640625" style="3"/>
+    <col min="13825" max="13828" width="2.4140625" style="3" customWidth="1"/>
+    <col min="13829" max="13829" width="60" style="3" customWidth="1"/>
+    <col min="13830" max="13830" width="3.1640625" style="3" customWidth="1"/>
+    <col min="13831" max="13831" width="6.6640625" style="3" customWidth="1"/>
+    <col min="13832" max="14080" width="8.1640625" style="3"/>
+    <col min="14081" max="14084" width="2.4140625" style="3" customWidth="1"/>
+    <col min="14085" max="14085" width="60" style="3" customWidth="1"/>
+    <col min="14086" max="14086" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14087" max="14087" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14088" max="14336" width="8.1640625" style="3"/>
+    <col min="14337" max="14340" width="2.4140625" style="3" customWidth="1"/>
+    <col min="14341" max="14341" width="60" style="3" customWidth="1"/>
+    <col min="14342" max="14342" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14343" max="14343" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14344" max="14592" width="8.1640625" style="3"/>
+    <col min="14593" max="14596" width="2.4140625" style="3" customWidth="1"/>
+    <col min="14597" max="14597" width="60" style="3" customWidth="1"/>
+    <col min="14598" max="14598" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14599" max="14599" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14600" max="14848" width="8.1640625" style="3"/>
+    <col min="14849" max="14852" width="2.4140625" style="3" customWidth="1"/>
+    <col min="14853" max="14853" width="60" style="3" customWidth="1"/>
+    <col min="14854" max="14854" width="3.1640625" style="3" customWidth="1"/>
+    <col min="14855" max="14855" width="6.6640625" style="3" customWidth="1"/>
+    <col min="14856" max="15104" width="8.1640625" style="3"/>
+    <col min="15105" max="15108" width="2.4140625" style="3" customWidth="1"/>
+    <col min="15109" max="15109" width="60" style="3" customWidth="1"/>
+    <col min="15110" max="15110" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15111" max="15111" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15112" max="15360" width="8.1640625" style="3"/>
+    <col min="15361" max="15364" width="2.4140625" style="3" customWidth="1"/>
+    <col min="15365" max="15365" width="60" style="3" customWidth="1"/>
+    <col min="15366" max="15366" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15367" max="15367" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15368" max="15616" width="8.1640625" style="3"/>
+    <col min="15617" max="15620" width="2.4140625" style="3" customWidth="1"/>
+    <col min="15621" max="15621" width="60" style="3" customWidth="1"/>
+    <col min="15622" max="15622" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15623" max="15623" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15624" max="15872" width="8.1640625" style="3"/>
+    <col min="15873" max="15876" width="2.4140625" style="3" customWidth="1"/>
+    <col min="15877" max="15877" width="60" style="3" customWidth="1"/>
+    <col min="15878" max="15878" width="3.1640625" style="3" customWidth="1"/>
+    <col min="15879" max="15879" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15880" max="16128" width="8.1640625" style="3"/>
+    <col min="16129" max="16132" width="2.4140625" style="3" customWidth="1"/>
+    <col min="16133" max="16133" width="60" style="3" customWidth="1"/>
+    <col min="16134" max="16134" width="3.1640625" style="3" customWidth="1"/>
+    <col min="16135" max="16135" width="6.6640625" style="3" customWidth="1"/>
+    <col min="16136" max="16384" width="8.1640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="4.5" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A4" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A5" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A6" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A7" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="4.5" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" ht="3" customHeight="1" thickTop="1"/>
+    <row r="11" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:7" s="9" customFormat="1" ht="4.5" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="1:7" ht="3" customHeight="1" thickTop="1">
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="35"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="35"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="49"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="49"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="33"/>
+      <c r="G22" s="49"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="49"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="49"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="33"/>
+      <c r="G25" s="49"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="35"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="49"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+    </row>
+    <row r="29" spans="1:7" ht="4.5" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A30" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+    </row>
+    <row r="31" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A31" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+    </row>
+    <row r="32" spans="1:7" ht="4.5" customHeight="1">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1" thickTop="1">
+      <c r="A34" s="45"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+    </row>
+    <row r="37" spans="1:7" ht="4.5" customHeight="1">
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A30:C30"/>
+  </mergeCells>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A0FACD-B6C3-47C2-9B4B-5459CCD3D95E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2632,11 +3646,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>